<commit_message>
adds sheet for every unique asset id
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,6 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="Total" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="p1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="p2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="p3" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W58"/>
+  <dimension ref="A1:S58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,85 +469,65 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Share 1</t>
+          <t>Note</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Share 2</t>
+          <t>Referrer</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Payment Type</t>
+          <t>Description</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Payment Provider</t>
+          <t>Customer ID</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Note</t>
+          <t>Customer UUID</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Referrer</t>
+          <t>Customer Email</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Description</t>
+          <t>Customer Name</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Customer ID</t>
+          <t>Voucher Code</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Customer UUID</t>
+          <t>Voucher Discount</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Customer Email</t>
+          <t>Country</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Customer Name</t>
+          <t>Created At</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Voucher Code</t>
+          <t>Client ID</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Voucher Discount</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Country</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Created At</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>Client ID</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Payment Tool Token</t>
         </is>
@@ -577,57 +560,36 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G2" t="n">
-        <v>6.732</v>
-      </c>
-      <c r="H2" t="n">
-        <v>125.268</v>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>https://www.virtualelvisweek.com/legacy/index.html</t>
+        </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>https://www.virtualelvisweek.com/legacy/index.html</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
           <t>Elvis Week Legacy Pass- 5 Live Legacy Pass Events + 1 Week VOD Each - $130 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N2" t="n">
+      <c r="J2" t="n">
         <v>57</v>
       </c>
-      <c r="O2" t="n">
+      <c r="K2" t="n">
         <v>57</v>
       </c>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>Ireland</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>7/7/22 20:56</t>
         </is>
       </c>
-      <c r="V2" t="n">
-        <v>0</v>
-      </c>
-      <c r="W2" t="inlineStr">
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="inlineStr">
         <is>
           <t>ch_</t>
         </is>
@@ -660,57 +622,36 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G3" t="n">
-        <v>11.577</v>
-      </c>
-      <c r="H3" t="n">
-        <v>215.423</v>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>https://virtualelvisweek.com/superfan/index.html</t>
+        </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>https://virtualelvisweek.com/superfan/index.html</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N3" t="n">
+      <c r="J3" t="n">
         <v>56</v>
       </c>
-      <c r="O3" t="n">
+      <c r="K3" t="n">
         <v>56</v>
       </c>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>Netherlands</t>
         </is>
       </c>
-      <c r="U3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>7/7/22 20:48</t>
         </is>
       </c>
-      <c r="V3" t="n">
-        <v>0</v>
-      </c>
-      <c r="W3" t="inlineStr">
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="inlineStr">
         <is>
           <t>ch_</t>
         </is>
@@ -743,59 +684,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr">
-        <is>
           <t>Elvis Week Legacy Pass- 5 Live Legacy Pass Events + 1 Week VOD Each - $130 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N4" t="n">
+      <c r="J4" t="n">
         <v>55</v>
       </c>
+      <c r="K4" t="n">
+        <v>55</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O4" t="n">
-        <v>55</v>
-      </c>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S4" t="n">
         <v>100</v>
       </c>
-      <c r="T4" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t>North Macedonia</t>
         </is>
       </c>
-      <c r="U4" t="inlineStr">
+      <c r="Q4" t="inlineStr">
         <is>
           <t>7/7/22 20:39</t>
         </is>
       </c>
-      <c r="V4" t="n">
-        <v>0</v>
-      </c>
-      <c r="W4" t="inlineStr">
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -828,57 +754,36 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G5" t="n">
-        <v>6.732</v>
-      </c>
-      <c r="H5" t="n">
-        <v>125.268</v>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>http://www.virtualelvisweek.com/legacy/index.html</t>
+        </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>http://www.virtualelvisweek.com/legacy/index.html</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
           <t>Elvis Week Legacy Pass- 5 Live Legacy Pass Events + 1 Week VOD Each - $130 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N5" t="n">
+      <c r="J5" t="n">
         <v>54</v>
       </c>
-      <c r="O5" t="n">
+      <c r="K5" t="n">
         <v>54</v>
       </c>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
-      <c r="T5" t="inlineStr">
+      <c r="P5" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U5" t="inlineStr">
+      <c r="Q5" t="inlineStr">
         <is>
           <t>7/7/22 20:27</t>
         </is>
       </c>
-      <c r="V5" t="n">
-        <v>0</v>
-      </c>
-      <c r="W5" t="inlineStr">
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="inlineStr">
         <is>
           <t>ch_</t>
         </is>
@@ -911,57 +816,36 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G6" t="n">
-        <v>11.577</v>
-      </c>
-      <c r="H6" t="n">
-        <v>215.423</v>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>http://www.virtualelvisweek.com/superfan/index.html</t>
+        </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>http://www.virtualelvisweek.com/superfan/index.html</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N6" t="n">
+      <c r="J6" t="n">
         <v>53</v>
       </c>
-      <c r="O6" t="n">
+      <c r="K6" t="n">
         <v>53</v>
       </c>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr"/>
-      <c r="T6" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U6" t="inlineStr">
+      <c r="Q6" t="inlineStr">
         <is>
           <t>7/7/22 20:17</t>
         </is>
       </c>
-      <c r="V6" t="n">
-        <v>0</v>
-      </c>
-      <c r="W6" t="inlineStr">
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="inlineStr">
         <is>
           <t>ch_</t>
         </is>
@@ -994,57 +878,36 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G7" t="n">
-        <v>6.732</v>
-      </c>
-      <c r="H7" t="n">
-        <v>125.268</v>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>https://virtualelvisweek.com/artisttribute/index.html</t>
+        </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>https://virtualelvisweek.com/artisttribute/index.html</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
           <t>Elvis Week Tribute Pass- 4 Live Tribute Pass Events + 1 Week  VOD Each - $130 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N7" t="n">
+      <c r="J7" t="n">
         <v>52</v>
       </c>
-      <c r="O7" t="n">
+      <c r="K7" t="n">
         <v>52</v>
       </c>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
-      <c r="T7" t="inlineStr">
+      <c r="P7" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U7" t="inlineStr">
+      <c r="Q7" t="inlineStr">
         <is>
           <t>7/7/22 20:10</t>
         </is>
       </c>
-      <c r="V7" t="n">
-        <v>0</v>
-      </c>
-      <c r="W7" t="inlineStr">
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="inlineStr">
         <is>
           <t>ch_</t>
         </is>
@@ -1077,57 +940,36 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G8" t="n">
-        <v>11.577</v>
-      </c>
-      <c r="H8" t="n">
-        <v>215.423</v>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>http://www.virtualelvisweek.com/superfan/index.html</t>
+        </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>http://www.virtualelvisweek.com/superfan/index.html</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N8" t="n">
+      <c r="J8" t="n">
         <v>51</v>
       </c>
-      <c r="O8" t="n">
+      <c r="K8" t="n">
         <v>51</v>
       </c>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr"/>
-      <c r="T8" t="inlineStr">
+      <c r="P8" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U8" t="inlineStr">
+      <c r="Q8" t="inlineStr">
         <is>
           <t>7/7/22 19:55</t>
         </is>
       </c>
-      <c r="V8" t="n">
-        <v>0</v>
-      </c>
-      <c r="W8" t="inlineStr">
+      <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="inlineStr">
         <is>
           <t>ch_</t>
         </is>
@@ -1160,57 +1002,36 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G9" t="n">
-        <v>11.577</v>
-      </c>
-      <c r="H9" t="n">
-        <v>215.423</v>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>http://www.virtualelvisweek.com/superfan/index.html</t>
+        </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>http://www.virtualelvisweek.com/superfan/index.html</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N9" t="n">
+      <c r="J9" t="n">
         <v>50</v>
       </c>
-      <c r="O9" t="n">
+      <c r="K9" t="n">
         <v>50</v>
       </c>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr"/>
-      <c r="T9" t="inlineStr">
+      <c r="P9" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U9" t="inlineStr">
+      <c r="Q9" t="inlineStr">
         <is>
           <t>7/7/22 19:55</t>
         </is>
       </c>
-      <c r="V9" t="n">
-        <v>0</v>
-      </c>
-      <c r="W9" t="inlineStr">
+      <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="inlineStr">
         <is>
           <t>ch_</t>
         </is>
@@ -1243,57 +1064,36 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G10" t="n">
-        <v>6.732</v>
-      </c>
-      <c r="H10" t="n">
-        <v>125.268</v>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>http://www.virtualelvisweek.com/legacy/index.html</t>
+        </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>http://www.virtualelvisweek.com/legacy/index.html</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
           <t>Elvis Week Legacy Pass- 5 Live Legacy Pass Events + 1 Week VOD Each - $130 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N10" t="n">
+      <c r="J10" t="n">
         <v>49</v>
       </c>
-      <c r="O10" t="n">
+      <c r="K10" t="n">
         <v>49</v>
       </c>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="inlineStr">
+      <c r="P10" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U10" t="inlineStr">
+      <c r="Q10" t="inlineStr">
         <is>
           <t>7/7/22 19:03</t>
         </is>
       </c>
-      <c r="V10" t="n">
-        <v>0</v>
-      </c>
-      <c r="W10" t="inlineStr">
+      <c r="R10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" t="inlineStr">
         <is>
           <t>ch_</t>
         </is>
@@ -1326,59 +1126,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr">
-        <is>
           <t>Elvis Week Legacy Pass- 5 Live Legacy Pass Events + 1 Week VOD Each - $130 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N11" t="n">
+      <c r="J11" t="n">
         <v>48</v>
       </c>
+      <c r="K11" t="n">
+        <v>48</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O11" t="n">
-        <v>48</v>
-      </c>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S11" t="n">
         <v>100</v>
       </c>
-      <c r="T11" t="inlineStr">
+      <c r="P11" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U11" t="inlineStr">
+      <c r="Q11" t="inlineStr">
         <is>
           <t>7/7/22 19:02</t>
         </is>
       </c>
-      <c r="V11" t="n">
-        <v>0</v>
-      </c>
-      <c r="W11" t="inlineStr">
+      <c r="R11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -1411,57 +1196,36 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G12" t="n">
-        <v>11.577</v>
-      </c>
-      <c r="H12" t="n">
-        <v>215.423</v>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>http://www.virtualelvisweek.com/superfan/index.html</t>
+        </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>http://www.virtualelvisweek.com/superfan/index.html</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N12" t="n">
+      <c r="J12" t="n">
         <v>47</v>
       </c>
-      <c r="O12" t="n">
+      <c r="K12" t="n">
         <v>47</v>
       </c>
-      <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr"/>
-      <c r="R12" t="inlineStr"/>
-      <c r="S12" t="inlineStr"/>
-      <c r="T12" t="inlineStr">
+      <c r="P12" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U12" t="inlineStr">
+      <c r="Q12" t="inlineStr">
         <is>
           <t>7/7/22 18:26</t>
         </is>
       </c>
-      <c r="V12" t="n">
-        <v>0</v>
-      </c>
-      <c r="W12" t="inlineStr">
+      <c r="R12" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" t="inlineStr">
         <is>
           <t>ch_</t>
         </is>
@@ -1494,59 +1258,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr">
-        <is>
           <t>Elvis Week Legacy Pass- 5 Live Legacy Pass Events + 1 Week VOD Each - $130 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N13" t="n">
+      <c r="J13" t="n">
         <v>46</v>
       </c>
+      <c r="K13" t="n">
+        <v>46</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O13" t="n">
-        <v>46</v>
-      </c>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S13" t="n">
         <v>100</v>
       </c>
-      <c r="T13" t="inlineStr">
+      <c r="P13" t="inlineStr">
         <is>
           <t>North Macedonia</t>
         </is>
       </c>
-      <c r="U13" t="inlineStr">
+      <c r="Q13" t="inlineStr">
         <is>
           <t>7/7/22 18:19</t>
         </is>
       </c>
-      <c r="V13" t="n">
-        <v>0</v>
-      </c>
-      <c r="W13" t="inlineStr">
+      <c r="R13" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -1579,57 +1328,36 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G14" t="n">
-        <v>6.732</v>
-      </c>
-      <c r="H14" t="n">
-        <v>125.268</v>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>http://www.virtualelvisweek.com/legacy/index.html</t>
+        </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>http://www.virtualelvisweek.com/legacy/index.html</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
           <t>Elvis Week Legacy Pass- 5 Live Legacy Pass Events + 1 Week VOD Each - $130 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N14" t="n">
+      <c r="J14" t="n">
         <v>45</v>
       </c>
-      <c r="O14" t="n">
+      <c r="K14" t="n">
         <v>45</v>
       </c>
-      <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="inlineStr"/>
-      <c r="S14" t="inlineStr"/>
-      <c r="T14" t="inlineStr">
+      <c r="P14" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U14" t="inlineStr">
+      <c r="Q14" t="inlineStr">
         <is>
           <t>7/7/22 17:57</t>
         </is>
       </c>
-      <c r="V14" t="n">
-        <v>0</v>
-      </c>
-      <c r="W14" t="inlineStr">
+      <c r="R14" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" t="inlineStr">
         <is>
           <t>ch_</t>
         </is>
@@ -1662,57 +1390,36 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G15" t="n">
-        <v>11.577</v>
-      </c>
-      <c r="H15" t="n">
-        <v>215.423</v>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>http://www.virtualelvisweek.com/superfan/index.html</t>
+        </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>http://www.virtualelvisweek.com/superfan/index.html</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N15" t="n">
+      <c r="J15" t="n">
         <v>44</v>
       </c>
-      <c r="O15" t="n">
+      <c r="K15" t="n">
         <v>44</v>
       </c>
-      <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="inlineStr"/>
-      <c r="R15" t="inlineStr"/>
-      <c r="S15" t="inlineStr"/>
-      <c r="T15" t="inlineStr">
+      <c r="P15" t="inlineStr">
         <is>
           <t>Ireland</t>
         </is>
       </c>
-      <c r="U15" t="inlineStr">
+      <c r="Q15" t="inlineStr">
         <is>
           <t>7/7/22 17:56</t>
         </is>
       </c>
-      <c r="V15" t="n">
-        <v>0</v>
-      </c>
-      <c r="W15" t="inlineStr">
+      <c r="R15" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" t="inlineStr">
         <is>
           <t>ch_</t>
         </is>
@@ -1745,57 +1452,36 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G16" t="n">
-        <v>11.577</v>
-      </c>
-      <c r="H16" t="n">
-        <v>215.423</v>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>https://virtualelvisweek.com/superfan/index.html</t>
+        </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>https://virtualelvisweek.com/superfan/index.html</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N16" t="n">
+      <c r="J16" t="n">
         <v>43</v>
       </c>
-      <c r="O16" t="n">
+      <c r="K16" t="n">
         <v>43</v>
       </c>
-      <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="inlineStr"/>
-      <c r="R16" t="inlineStr"/>
-      <c r="S16" t="inlineStr"/>
-      <c r="T16" t="inlineStr">
+      <c r="P16" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U16" t="inlineStr">
+      <c r="Q16" t="inlineStr">
         <is>
           <t>7/7/22 17:55</t>
         </is>
       </c>
-      <c r="V16" t="n">
-        <v>0</v>
-      </c>
-      <c r="W16" t="inlineStr">
+      <c r="R16" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" t="inlineStr">
         <is>
           <t>ch_</t>
         </is>
@@ -1828,57 +1514,36 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G17" t="n">
-        <v>11.577</v>
-      </c>
-      <c r="H17" t="n">
-        <v>215.423</v>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>http://www.virtualelvisweek.com/superfan/index.html</t>
+        </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>http://www.virtualelvisweek.com/superfan/index.html</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N17" t="n">
+      <c r="J17" t="n">
         <v>42</v>
       </c>
-      <c r="O17" t="n">
+      <c r="K17" t="n">
         <v>42</v>
       </c>
-      <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="inlineStr"/>
-      <c r="R17" t="inlineStr"/>
-      <c r="S17" t="inlineStr"/>
-      <c r="T17" t="inlineStr">
+      <c r="P17" t="inlineStr">
         <is>
           <t>United Kingdom</t>
         </is>
       </c>
-      <c r="U17" t="inlineStr">
+      <c r="Q17" t="inlineStr">
         <is>
           <t>7/7/22 17:52</t>
         </is>
       </c>
-      <c r="V17" t="n">
-        <v>0</v>
-      </c>
-      <c r="W17" t="inlineStr">
+      <c r="R17" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" t="inlineStr">
         <is>
           <t>ch_</t>
         </is>
@@ -1911,59 +1576,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr">
-        <is>
           <t>Elvis Week Legacy Pass- 5 Live Legacy Pass Events + 1 Week VOD Each - $130 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N18" t="n">
+      <c r="J18" t="n">
         <v>41</v>
       </c>
+      <c r="K18" t="n">
+        <v>41</v>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O18" t="n">
-        <v>41</v>
-      </c>
-      <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr"/>
-      <c r="R18" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S18" t="n">
         <v>100</v>
       </c>
-      <c r="T18" t="inlineStr">
+      <c r="P18" t="inlineStr">
         <is>
           <t>North Macedonia</t>
         </is>
       </c>
-      <c r="U18" t="inlineStr">
+      <c r="Q18" t="inlineStr">
         <is>
           <t>7/7/22 17:45</t>
         </is>
       </c>
-      <c r="V18" t="n">
-        <v>0</v>
-      </c>
-      <c r="W18" t="inlineStr">
+      <c r="R18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -1996,59 +1646,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N19" t="n">
+      <c r="J19" t="n">
         <v>40</v>
       </c>
+      <c r="K19" t="n">
+        <v>40</v>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O19" t="n">
-        <v>40</v>
-      </c>
-      <c r="P19" t="inlineStr"/>
-      <c r="Q19" t="inlineStr"/>
-      <c r="R19" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S19" t="n">
         <v>100</v>
       </c>
-      <c r="T19" t="inlineStr">
+      <c r="P19" t="inlineStr">
         <is>
           <t>North Macedonia</t>
         </is>
       </c>
-      <c r="U19" t="inlineStr">
+      <c r="Q19" t="inlineStr">
         <is>
           <t>7/7/22 17:40</t>
         </is>
       </c>
-      <c r="V19" t="n">
-        <v>0</v>
-      </c>
-      <c r="W19" t="inlineStr">
+      <c r="R19" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -2081,57 +1716,36 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G20" t="n">
-        <v>6.732</v>
-      </c>
-      <c r="H20" t="n">
-        <v>125.268</v>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>http://www.virtualelvisweek.com/legacy/index.html</t>
+        </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr"/>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>http://www.virtualelvisweek.com/legacy/index.html</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr">
-        <is>
           <t>Elvis Week Legacy Pass- 5 Live Legacy Pass Events + 1 Week VOD Each - $130 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N20" t="n">
+      <c r="J20" t="n">
         <v>39</v>
       </c>
-      <c r="O20" t="n">
+      <c r="K20" t="n">
         <v>39</v>
       </c>
-      <c r="P20" t="inlineStr"/>
-      <c r="Q20" t="inlineStr"/>
-      <c r="R20" t="inlineStr"/>
-      <c r="S20" t="inlineStr"/>
-      <c r="T20" t="inlineStr">
+      <c r="P20" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U20" t="inlineStr">
+      <c r="Q20" t="inlineStr">
         <is>
           <t>7/7/22 17:29</t>
         </is>
       </c>
-      <c r="V20" t="n">
-        <v>0</v>
-      </c>
-      <c r="W20" t="inlineStr">
+      <c r="R20" t="n">
+        <v>0</v>
+      </c>
+      <c r="S20" t="inlineStr">
         <is>
           <t>ch_</t>
         </is>
@@ -2164,57 +1778,36 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G21" t="n">
-        <v>11.577</v>
-      </c>
-      <c r="H21" t="n">
-        <v>215.423</v>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>https://virtualelvisweek.com/superfan/index.html</t>
+        </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>https://virtualelvisweek.com/superfan/index.html</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N21" t="n">
+      <c r="J21" t="n">
         <v>38</v>
       </c>
-      <c r="O21" t="n">
+      <c r="K21" t="n">
         <v>38</v>
       </c>
-      <c r="P21" t="inlineStr"/>
-      <c r="Q21" t="inlineStr"/>
-      <c r="R21" t="inlineStr"/>
-      <c r="S21" t="inlineStr"/>
-      <c r="T21" t="inlineStr">
+      <c r="P21" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U21" t="inlineStr">
+      <c r="Q21" t="inlineStr">
         <is>
           <t>7/7/22 17:24</t>
         </is>
       </c>
-      <c r="V21" t="n">
-        <v>0</v>
-      </c>
-      <c r="W21" t="inlineStr">
+      <c r="R21" t="n">
+        <v>0</v>
+      </c>
+      <c r="S21" t="inlineStr">
         <is>
           <t>ch_</t>
         </is>
@@ -2247,57 +1840,36 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G22" t="n">
-        <v>6.732</v>
-      </c>
-      <c r="H22" t="n">
-        <v>125.268</v>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>http://www.virtualelvisweek.com/artisttribute/index.html</t>
+        </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr"/>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>http://www.virtualelvisweek.com/artisttribute/index.html</t>
-        </is>
-      </c>
-      <c r="M22" t="inlineStr">
-        <is>
           <t>Elvis Week Tribute Pass- 4 Live Tribute Pass Events + 1 Week  VOD Each - $130 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N22" t="n">
+      <c r="J22" t="n">
         <v>37</v>
       </c>
-      <c r="O22" t="n">
+      <c r="K22" t="n">
         <v>37</v>
       </c>
-      <c r="P22" t="inlineStr"/>
-      <c r="Q22" t="inlineStr"/>
-      <c r="R22" t="inlineStr"/>
-      <c r="S22" t="inlineStr"/>
-      <c r="T22" t="inlineStr">
+      <c r="P22" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U22" t="inlineStr">
+      <c r="Q22" t="inlineStr">
         <is>
           <t>7/7/22 17:22</t>
         </is>
       </c>
-      <c r="V22" t="n">
-        <v>0</v>
-      </c>
-      <c r="W22" t="inlineStr">
+      <c r="R22" t="n">
+        <v>0</v>
+      </c>
+      <c r="S22" t="inlineStr">
         <is>
           <t>ch_</t>
         </is>
@@ -2330,57 +1902,36 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G23" t="n">
-        <v>11.577</v>
-      </c>
-      <c r="H23" t="n">
-        <v>215.423</v>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>http://www.virtualelvisweek.com/superfan/index.html</t>
+        </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>http://www.virtualelvisweek.com/superfan/index.html</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N23" t="n">
+      <c r="J23" t="n">
         <v>36</v>
       </c>
-      <c r="O23" t="n">
+      <c r="K23" t="n">
         <v>36</v>
       </c>
-      <c r="P23" t="inlineStr"/>
-      <c r="Q23" t="inlineStr"/>
-      <c r="R23" t="inlineStr"/>
-      <c r="S23" t="inlineStr"/>
-      <c r="T23" t="inlineStr">
+      <c r="P23" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U23" t="inlineStr">
+      <c r="Q23" t="inlineStr">
         <is>
           <t>7/7/22 17:21</t>
         </is>
       </c>
-      <c r="V23" t="n">
-        <v>0</v>
-      </c>
-      <c r="W23" t="inlineStr">
+      <c r="R23" t="n">
+        <v>0</v>
+      </c>
+      <c r="S23" t="inlineStr">
         <is>
           <t>ch_</t>
         </is>
@@ -2413,57 +1964,36 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G24" t="n">
-        <v>11.577</v>
-      </c>
-      <c r="H24" t="n">
-        <v>215.423</v>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>http://www.virtualelvisweek.com/superfan/index.html</t>
+        </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>http://www.virtualelvisweek.com/superfan/index.html</t>
-        </is>
-      </c>
-      <c r="M24" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N24" t="n">
+      <c r="J24" t="n">
         <v>35</v>
       </c>
-      <c r="O24" t="n">
+      <c r="K24" t="n">
         <v>35</v>
       </c>
-      <c r="P24" t="inlineStr"/>
-      <c r="Q24" t="inlineStr"/>
-      <c r="R24" t="inlineStr"/>
-      <c r="S24" t="inlineStr"/>
-      <c r="T24" t="inlineStr">
+      <c r="P24" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U24" t="inlineStr">
+      <c r="Q24" t="inlineStr">
         <is>
           <t>7/7/22 17:19</t>
         </is>
       </c>
-      <c r="V24" t="n">
-        <v>0</v>
-      </c>
-      <c r="W24" t="inlineStr">
+      <c r="R24" t="n">
+        <v>0</v>
+      </c>
+      <c r="S24" t="inlineStr">
         <is>
           <t>ch_</t>
         </is>
@@ -2496,57 +2026,36 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G25" t="n">
-        <v>11.577</v>
-      </c>
-      <c r="H25" t="n">
-        <v>215.423</v>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>http://www.virtualelvisweek.com/superfan/index.html</t>
+        </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr"/>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>http://www.virtualelvisweek.com/superfan/index.html</t>
-        </is>
-      </c>
-      <c r="M25" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N25" t="n">
+      <c r="J25" t="n">
         <v>34</v>
       </c>
-      <c r="O25" t="n">
+      <c r="K25" t="n">
         <v>34</v>
       </c>
-      <c r="P25" t="inlineStr"/>
-      <c r="Q25" t="inlineStr"/>
-      <c r="R25" t="inlineStr"/>
-      <c r="S25" t="inlineStr"/>
-      <c r="T25" t="inlineStr">
+      <c r="P25" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U25" t="inlineStr">
+      <c r="Q25" t="inlineStr">
         <is>
           <t>7/7/22 17:16</t>
         </is>
       </c>
-      <c r="V25" t="n">
-        <v>0</v>
-      </c>
-      <c r="W25" t="inlineStr">
+      <c r="R25" t="n">
+        <v>0</v>
+      </c>
+      <c r="S25" t="inlineStr">
         <is>
           <t>ch_</t>
         </is>
@@ -2579,57 +2088,36 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G26" t="n">
-        <v>6.732</v>
-      </c>
-      <c r="H26" t="n">
-        <v>125.268</v>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>https://www.virtualelvisweek.com/legacy/index.html</t>
+        </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr"/>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>https://www.virtualelvisweek.com/legacy/index.html</t>
-        </is>
-      </c>
-      <c r="M26" t="inlineStr">
-        <is>
           <t>Elvis Week Legacy Pass- 5 Live Legacy Pass Events + 1 Week VOD Each - $130 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N26" t="n">
+      <c r="J26" t="n">
         <v>33</v>
       </c>
-      <c r="O26" t="n">
+      <c r="K26" t="n">
         <v>33</v>
       </c>
-      <c r="P26" t="inlineStr"/>
-      <c r="Q26" t="inlineStr"/>
-      <c r="R26" t="inlineStr"/>
-      <c r="S26" t="inlineStr"/>
-      <c r="T26" t="inlineStr">
+      <c r="P26" t="inlineStr">
         <is>
           <t>Sweden</t>
         </is>
       </c>
-      <c r="U26" t="inlineStr">
+      <c r="Q26" t="inlineStr">
         <is>
           <t>7/7/22 16:47</t>
         </is>
       </c>
-      <c r="V26" t="n">
-        <v>0</v>
-      </c>
-      <c r="W26" t="inlineStr">
+      <c r="R26" t="n">
+        <v>0</v>
+      </c>
+      <c r="S26" t="inlineStr">
         <is>
           <t>ch_</t>
         </is>
@@ -2662,57 +2150,36 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G27" t="n">
-        <v>11.577</v>
-      </c>
-      <c r="H27" t="n">
-        <v>215.423</v>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>https://virtualelvisweek.com/superfan/index.html</t>
+        </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr"/>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>https://virtualelvisweek.com/superfan/index.html</t>
-        </is>
-      </c>
-      <c r="M27" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N27" t="n">
+      <c r="J27" t="n">
         <v>32</v>
       </c>
-      <c r="O27" t="n">
+      <c r="K27" t="n">
         <v>32</v>
       </c>
-      <c r="P27" t="inlineStr"/>
-      <c r="Q27" t="inlineStr"/>
-      <c r="R27" t="inlineStr"/>
-      <c r="S27" t="inlineStr"/>
-      <c r="T27" t="inlineStr">
+      <c r="P27" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U27" t="inlineStr">
+      <c r="Q27" t="inlineStr">
         <is>
           <t>7/7/22 16:46</t>
         </is>
       </c>
-      <c r="V27" t="n">
-        <v>0</v>
-      </c>
-      <c r="W27" t="inlineStr">
+      <c r="R27" t="n">
+        <v>0</v>
+      </c>
+      <c r="S27" t="inlineStr">
         <is>
           <t>ch_</t>
         </is>
@@ -2745,57 +2212,36 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G28" t="n">
-        <v>11.577</v>
-      </c>
-      <c r="H28" t="n">
-        <v>215.423</v>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>http://www.virtualelvisweek.com/superfan/index.html</t>
+        </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr"/>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>http://www.virtualelvisweek.com/superfan/index.html</t>
-        </is>
-      </c>
-      <c r="M28" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N28" t="n">
+      <c r="J28" t="n">
         <v>31</v>
       </c>
-      <c r="O28" t="n">
+      <c r="K28" t="n">
         <v>31</v>
       </c>
-      <c r="P28" t="inlineStr"/>
-      <c r="Q28" t="inlineStr"/>
-      <c r="R28" t="inlineStr"/>
-      <c r="S28" t="inlineStr"/>
-      <c r="T28" t="inlineStr">
+      <c r="P28" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U28" t="inlineStr">
+      <c r="Q28" t="inlineStr">
         <is>
           <t>7/7/22 16:36</t>
         </is>
       </c>
-      <c r="V28" t="n">
-        <v>0</v>
-      </c>
-      <c r="W28" t="inlineStr">
+      <c r="R28" t="n">
+        <v>0</v>
+      </c>
+      <c r="S28" t="inlineStr">
         <is>
           <t>ch_</t>
         </is>
@@ -2828,57 +2274,36 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G29" t="n">
-        <v>11.577</v>
-      </c>
-      <c r="H29" t="n">
-        <v>215.423</v>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>http://www.virtualelvisweek.com/superfan/index.html</t>
+        </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr"/>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>http://www.virtualelvisweek.com/superfan/index.html</t>
-        </is>
-      </c>
-      <c r="M29" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N29" t="n">
+      <c r="J29" t="n">
         <v>30</v>
       </c>
-      <c r="O29" t="n">
+      <c r="K29" t="n">
         <v>30</v>
       </c>
-      <c r="P29" t="inlineStr"/>
-      <c r="Q29" t="inlineStr"/>
-      <c r="R29" t="inlineStr"/>
-      <c r="S29" t="inlineStr"/>
-      <c r="T29" t="inlineStr">
+      <c r="P29" t="inlineStr">
         <is>
           <t>Canada</t>
         </is>
       </c>
-      <c r="U29" t="inlineStr">
+      <c r="Q29" t="inlineStr">
         <is>
           <t>7/7/22 16:29</t>
         </is>
       </c>
-      <c r="V29" t="n">
-        <v>0</v>
-      </c>
-      <c r="W29" t="inlineStr">
+      <c r="R29" t="n">
+        <v>0</v>
+      </c>
+      <c r="S29" t="inlineStr">
         <is>
           <t>ch_</t>
         </is>
@@ -2911,57 +2336,36 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G30" t="n">
-        <v>11.577</v>
-      </c>
-      <c r="H30" t="n">
-        <v>215.423</v>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>http://www.virtualelvisweek.com/superfan/index.html</t>
+        </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K30" t="inlineStr"/>
-      <c r="L30" t="inlineStr">
-        <is>
-          <t>http://www.virtualelvisweek.com/superfan/index.html</t>
-        </is>
-      </c>
-      <c r="M30" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N30" t="n">
+      <c r="J30" t="n">
         <v>29</v>
       </c>
-      <c r="O30" t="n">
+      <c r="K30" t="n">
         <v>29</v>
       </c>
-      <c r="P30" t="inlineStr"/>
-      <c r="Q30" t="inlineStr"/>
-      <c r="R30" t="inlineStr"/>
-      <c r="S30" t="inlineStr"/>
-      <c r="T30" t="inlineStr">
+      <c r="P30" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U30" t="inlineStr">
+      <c r="Q30" t="inlineStr">
         <is>
           <t>7/7/22 16:18</t>
         </is>
       </c>
-      <c r="V30" t="n">
-        <v>0</v>
-      </c>
-      <c r="W30" t="inlineStr">
+      <c r="R30" t="n">
+        <v>0</v>
+      </c>
+      <c r="S30" t="inlineStr">
         <is>
           <t>ch_</t>
         </is>
@@ -2994,57 +2398,36 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G31" t="n">
-        <v>6.732</v>
-      </c>
-      <c r="H31" t="n">
-        <v>125.268</v>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>http://www.virtualelvisweek.com/artisttribute/index.html</t>
+        </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K31" t="inlineStr"/>
-      <c r="L31" t="inlineStr">
-        <is>
-          <t>http://www.virtualelvisweek.com/artisttribute/index.html</t>
-        </is>
-      </c>
-      <c r="M31" t="inlineStr">
-        <is>
           <t>Elvis Week Tribute Pass- 4 Live Tribute Pass Events + 1 Week  VOD Each - $130 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N31" t="n">
+      <c r="J31" t="n">
         <v>28</v>
       </c>
-      <c r="O31" t="n">
+      <c r="K31" t="n">
         <v>28</v>
       </c>
-      <c r="P31" t="inlineStr"/>
-      <c r="Q31" t="inlineStr"/>
-      <c r="R31" t="inlineStr"/>
-      <c r="S31" t="inlineStr"/>
-      <c r="T31" t="inlineStr">
+      <c r="P31" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U31" t="inlineStr">
+      <c r="Q31" t="inlineStr">
         <is>
           <t>7/7/22 16:17</t>
         </is>
       </c>
-      <c r="V31" t="n">
-        <v>0</v>
-      </c>
-      <c r="W31" t="inlineStr">
+      <c r="R31" t="n">
+        <v>0</v>
+      </c>
+      <c r="S31" t="inlineStr">
         <is>
           <t>ch_</t>
         </is>
@@ -3077,57 +2460,36 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G32" t="n">
-        <v>11.577</v>
-      </c>
-      <c r="H32" t="n">
-        <v>215.423</v>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>http://www.virtualelvisweek.com/superfan/index.html</t>
+        </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K32" t="inlineStr"/>
-      <c r="L32" t="inlineStr">
-        <is>
-          <t>http://www.virtualelvisweek.com/superfan/index.html</t>
-        </is>
-      </c>
-      <c r="M32" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N32" t="n">
+      <c r="J32" t="n">
         <v>27</v>
       </c>
-      <c r="O32" t="n">
+      <c r="K32" t="n">
         <v>27</v>
       </c>
-      <c r="P32" t="inlineStr"/>
-      <c r="Q32" t="inlineStr"/>
-      <c r="R32" t="inlineStr"/>
-      <c r="S32" t="inlineStr"/>
-      <c r="T32" t="inlineStr">
+      <c r="P32" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U32" t="inlineStr">
+      <c r="Q32" t="inlineStr">
         <is>
           <t>7/7/22 15:49</t>
         </is>
       </c>
-      <c r="V32" t="n">
-        <v>0</v>
-      </c>
-      <c r="W32" t="inlineStr">
+      <c r="R32" t="n">
+        <v>0</v>
+      </c>
+      <c r="S32" t="inlineStr">
         <is>
           <t>ch_</t>
         </is>
@@ -3160,59 +2522,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr"/>
-      <c r="H33" t="inlineStr"/>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L33" t="inlineStr"/>
-      <c r="M33" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N33" t="n">
+      <c r="J33" t="n">
         <v>26</v>
       </c>
+      <c r="K33" t="n">
+        <v>26</v>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O33" t="n">
-        <v>26</v>
-      </c>
-      <c r="P33" t="inlineStr"/>
-      <c r="Q33" t="inlineStr"/>
-      <c r="R33" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S33" t="n">
         <v>100</v>
       </c>
-      <c r="T33" t="inlineStr">
+      <c r="P33" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U33" t="inlineStr">
+      <c r="Q33" t="inlineStr">
         <is>
           <t>7/6/22 18:53</t>
         </is>
       </c>
-      <c r="V33" t="n">
-        <v>0</v>
-      </c>
-      <c r="W33" t="inlineStr">
+      <c r="R33" t="n">
+        <v>0</v>
+      </c>
+      <c r="S33" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -3245,59 +2592,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr"/>
-      <c r="H34" t="inlineStr"/>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L34" t="inlineStr"/>
-      <c r="M34" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N34" t="n">
+      <c r="J34" t="n">
         <v>25</v>
       </c>
+      <c r="K34" t="n">
+        <v>25</v>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O34" t="n">
-        <v>25</v>
-      </c>
-      <c r="P34" t="inlineStr"/>
-      <c r="Q34" t="inlineStr"/>
-      <c r="R34" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S34" t="n">
         <v>100</v>
       </c>
-      <c r="T34" t="inlineStr">
+      <c r="P34" t="inlineStr">
         <is>
           <t>North Macedonia</t>
         </is>
       </c>
-      <c r="U34" t="inlineStr">
+      <c r="Q34" t="inlineStr">
         <is>
           <t>7/6/22 18:16</t>
         </is>
       </c>
-      <c r="V34" t="n">
-        <v>0</v>
-      </c>
-      <c r="W34" t="inlineStr">
+      <c r="R34" t="n">
+        <v>0</v>
+      </c>
+      <c r="S34" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -3330,59 +2662,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L35" t="inlineStr"/>
-      <c r="M35" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N35" t="n">
+      <c r="J35" t="n">
         <v>24</v>
       </c>
+      <c r="K35" t="n">
+        <v>24</v>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O35" t="n">
-        <v>24</v>
-      </c>
-      <c r="P35" t="inlineStr"/>
-      <c r="Q35" t="inlineStr"/>
-      <c r="R35" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S35" t="n">
         <v>100</v>
       </c>
-      <c r="T35" t="inlineStr">
+      <c r="P35" t="inlineStr">
         <is>
           <t>North Macedonia</t>
         </is>
       </c>
-      <c r="U35" t="inlineStr">
+      <c r="Q35" t="inlineStr">
         <is>
           <t>7/6/22 18:05</t>
         </is>
       </c>
-      <c r="V35" t="n">
-        <v>0</v>
-      </c>
-      <c r="W35" t="inlineStr">
+      <c r="R35" t="n">
+        <v>0</v>
+      </c>
+      <c r="S35" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -3415,59 +2732,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr"/>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L36" t="inlineStr"/>
-      <c r="M36" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N36" t="n">
+      <c r="J36" t="n">
         <v>23</v>
       </c>
+      <c r="K36" t="n">
+        <v>23</v>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O36" t="n">
-        <v>23</v>
-      </c>
-      <c r="P36" t="inlineStr"/>
-      <c r="Q36" t="inlineStr"/>
-      <c r="R36" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S36" t="n">
         <v>100</v>
       </c>
-      <c r="T36" t="inlineStr">
+      <c r="P36" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U36" t="inlineStr">
+      <c r="Q36" t="inlineStr">
         <is>
           <t>7/6/22 18:04</t>
         </is>
       </c>
-      <c r="V36" t="n">
-        <v>0</v>
-      </c>
-      <c r="W36" t="inlineStr">
+      <c r="R36" t="n">
+        <v>0</v>
+      </c>
+      <c r="S36" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -3500,59 +2802,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G37" t="inlineStr"/>
-      <c r="H37" t="inlineStr"/>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L37" t="inlineStr"/>
-      <c r="M37" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N37" t="n">
+      <c r="J37" t="n">
         <v>22</v>
       </c>
+      <c r="K37" t="n">
+        <v>22</v>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O37" t="n">
-        <v>22</v>
-      </c>
-      <c r="P37" t="inlineStr"/>
-      <c r="Q37" t="inlineStr"/>
-      <c r="R37" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S37" t="n">
         <v>100</v>
       </c>
-      <c r="T37" t="inlineStr">
+      <c r="P37" t="inlineStr">
         <is>
           <t>North Macedonia</t>
         </is>
       </c>
-      <c r="U37" t="inlineStr">
+      <c r="Q37" t="inlineStr">
         <is>
           <t>7/6/22 18:02</t>
         </is>
       </c>
-      <c r="V37" t="n">
-        <v>0</v>
-      </c>
-      <c r="W37" t="inlineStr">
+      <c r="R37" t="n">
+        <v>0</v>
+      </c>
+      <c r="S37" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -3585,59 +2872,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G38" t="inlineStr"/>
-      <c r="H38" t="inlineStr"/>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L38" t="inlineStr"/>
-      <c r="M38" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N38" t="n">
+      <c r="J38" t="n">
         <v>21</v>
       </c>
+      <c r="K38" t="n">
+        <v>21</v>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O38" t="n">
-        <v>21</v>
-      </c>
-      <c r="P38" t="inlineStr"/>
-      <c r="Q38" t="inlineStr"/>
-      <c r="R38" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S38" t="n">
         <v>100</v>
       </c>
-      <c r="T38" t="inlineStr">
+      <c r="P38" t="inlineStr">
         <is>
           <t>North Macedonia</t>
         </is>
       </c>
-      <c r="U38" t="inlineStr">
+      <c r="Q38" t="inlineStr">
         <is>
           <t>7/6/22 17:58</t>
         </is>
       </c>
-      <c r="V38" t="n">
-        <v>0</v>
-      </c>
-      <c r="W38" t="inlineStr">
+      <c r="R38" t="n">
+        <v>0</v>
+      </c>
+      <c r="S38" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -3670,59 +2942,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G39" t="inlineStr"/>
-      <c r="H39" t="inlineStr"/>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L39" t="inlineStr"/>
-      <c r="M39" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N39" t="n">
+      <c r="J39" t="n">
         <v>20</v>
       </c>
+      <c r="K39" t="n">
+        <v>20</v>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O39" t="n">
-        <v>20</v>
-      </c>
-      <c r="P39" t="inlineStr"/>
-      <c r="Q39" t="inlineStr"/>
-      <c r="R39" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S39" t="n">
         <v>100</v>
       </c>
-      <c r="T39" t="inlineStr">
+      <c r="P39" t="inlineStr">
         <is>
           <t>North Macedonia</t>
         </is>
       </c>
-      <c r="U39" t="inlineStr">
+      <c r="Q39" t="inlineStr">
         <is>
           <t>7/6/22 17:56</t>
         </is>
       </c>
-      <c r="V39" t="n">
-        <v>0</v>
-      </c>
-      <c r="W39" t="inlineStr">
+      <c r="R39" t="n">
+        <v>0</v>
+      </c>
+      <c r="S39" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -3755,59 +3012,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr"/>
-      <c r="H40" t="inlineStr"/>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L40" t="inlineStr"/>
-      <c r="M40" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N40" t="n">
+      <c r="J40" t="n">
         <v>19</v>
       </c>
+      <c r="K40" t="n">
+        <v>19</v>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O40" t="n">
-        <v>19</v>
-      </c>
-      <c r="P40" t="inlineStr"/>
-      <c r="Q40" t="inlineStr"/>
-      <c r="R40" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S40" t="n">
         <v>100</v>
       </c>
-      <c r="T40" t="inlineStr">
+      <c r="P40" t="inlineStr">
         <is>
           <t>North Macedonia</t>
         </is>
       </c>
-      <c r="U40" t="inlineStr">
+      <c r="Q40" t="inlineStr">
         <is>
           <t>7/6/22 17:53</t>
         </is>
       </c>
-      <c r="V40" t="n">
-        <v>0</v>
-      </c>
-      <c r="W40" t="inlineStr">
+      <c r="R40" t="n">
+        <v>0</v>
+      </c>
+      <c r="S40" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -3840,59 +3082,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G41" t="inlineStr"/>
-      <c r="H41" t="inlineStr"/>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K41" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L41" t="inlineStr"/>
-      <c r="M41" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N41" t="n">
+      <c r="J41" t="n">
         <v>18</v>
       </c>
+      <c r="K41" t="n">
+        <v>18</v>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O41" t="n">
-        <v>18</v>
-      </c>
-      <c r="P41" t="inlineStr"/>
-      <c r="Q41" t="inlineStr"/>
-      <c r="R41" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S41" t="n">
         <v>100</v>
       </c>
-      <c r="T41" t="inlineStr">
+      <c r="P41" t="inlineStr">
         <is>
           <t>North Macedonia</t>
         </is>
       </c>
-      <c r="U41" t="inlineStr">
+      <c r="Q41" t="inlineStr">
         <is>
           <t>7/6/22 17:51</t>
         </is>
       </c>
-      <c r="V41" t="n">
-        <v>0</v>
-      </c>
-      <c r="W41" t="inlineStr">
+      <c r="R41" t="n">
+        <v>0</v>
+      </c>
+      <c r="S41" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -3925,59 +3152,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G42" t="inlineStr"/>
-      <c r="H42" t="inlineStr"/>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L42" t="inlineStr"/>
-      <c r="M42" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N42" t="n">
+      <c r="J42" t="n">
         <v>17</v>
       </c>
+      <c r="K42" t="n">
+        <v>17</v>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O42" t="n">
-        <v>17</v>
-      </c>
-      <c r="P42" t="inlineStr"/>
-      <c r="Q42" t="inlineStr"/>
-      <c r="R42" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S42" t="n">
         <v>100</v>
       </c>
-      <c r="T42" t="inlineStr">
+      <c r="P42" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U42" t="inlineStr">
+      <c r="Q42" t="inlineStr">
         <is>
           <t>7/6/22 17:51</t>
         </is>
       </c>
-      <c r="V42" t="n">
-        <v>0</v>
-      </c>
-      <c r="W42" t="inlineStr">
+      <c r="R42" t="n">
+        <v>0</v>
+      </c>
+      <c r="S42" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -4010,59 +3222,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="inlineStr"/>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K43" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L43" t="inlineStr"/>
-      <c r="M43" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N43" t="n">
+      <c r="J43" t="n">
         <v>16</v>
       </c>
+      <c r="K43" t="n">
+        <v>16</v>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O43" t="n">
-        <v>16</v>
-      </c>
-      <c r="P43" t="inlineStr"/>
-      <c r="Q43" t="inlineStr"/>
-      <c r="R43" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S43" t="n">
         <v>100</v>
       </c>
-      <c r="T43" t="inlineStr">
+      <c r="P43" t="inlineStr">
         <is>
           <t>North Macedonia</t>
         </is>
       </c>
-      <c r="U43" t="inlineStr">
+      <c r="Q43" t="inlineStr">
         <is>
           <t>7/6/22 17:49</t>
         </is>
       </c>
-      <c r="V43" t="n">
-        <v>0</v>
-      </c>
-      <c r="W43" t="inlineStr">
+      <c r="R43" t="n">
+        <v>0</v>
+      </c>
+      <c r="S43" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -4095,59 +3292,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G44" t="inlineStr"/>
-      <c r="H44" t="inlineStr"/>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L44" t="inlineStr"/>
-      <c r="M44" t="inlineStr">
-        <is>
           <t>Elvis Week Legacy Pass- 5 Live Legacy Pass Events + 1 Week VOD Each - $130 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N44" t="n">
+      <c r="J44" t="n">
         <v>15</v>
       </c>
+      <c r="K44" t="n">
+        <v>15</v>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O44" t="n">
-        <v>15</v>
-      </c>
-      <c r="P44" t="inlineStr"/>
-      <c r="Q44" t="inlineStr"/>
-      <c r="R44" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S44" t="n">
         <v>100</v>
       </c>
-      <c r="T44" t="inlineStr">
+      <c r="P44" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U44" t="inlineStr">
+      <c r="Q44" t="inlineStr">
         <is>
           <t>7/6/22 17:15</t>
         </is>
       </c>
-      <c r="V44" t="n">
-        <v>0</v>
-      </c>
-      <c r="W44" t="inlineStr">
+      <c r="R44" t="n">
+        <v>0</v>
+      </c>
+      <c r="S44" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -4180,59 +3362,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G45" t="inlineStr"/>
-      <c r="H45" t="inlineStr"/>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L45" t="inlineStr"/>
-      <c r="M45" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N45" t="n">
+      <c r="J45" t="n">
         <v>14</v>
       </c>
+      <c r="K45" t="n">
+        <v>14</v>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O45" t="n">
-        <v>14</v>
-      </c>
-      <c r="P45" t="inlineStr"/>
-      <c r="Q45" t="inlineStr"/>
-      <c r="R45" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S45" t="n">
         <v>100</v>
       </c>
-      <c r="T45" t="inlineStr">
+      <c r="P45" t="inlineStr">
         <is>
           <t>North Macedonia</t>
         </is>
       </c>
-      <c r="U45" t="inlineStr">
+      <c r="Q45" t="inlineStr">
         <is>
           <t>7/6/22 17:09</t>
         </is>
       </c>
-      <c r="V45" t="n">
-        <v>0</v>
-      </c>
-      <c r="W45" t="inlineStr">
+      <c r="R45" t="n">
+        <v>0</v>
+      </c>
+      <c r="S45" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -4265,59 +3432,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G46" t="inlineStr"/>
-      <c r="H46" t="inlineStr"/>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L46" t="inlineStr"/>
-      <c r="M46" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N46" t="n">
+      <c r="J46" t="n">
         <v>13</v>
       </c>
+      <c r="K46" t="n">
+        <v>13</v>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O46" t="n">
-        <v>13</v>
-      </c>
-      <c r="P46" t="inlineStr"/>
-      <c r="Q46" t="inlineStr"/>
-      <c r="R46" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S46" t="n">
         <v>100</v>
       </c>
-      <c r="T46" t="inlineStr">
+      <c r="P46" t="inlineStr">
         <is>
           <t>North Macedonia</t>
         </is>
       </c>
-      <c r="U46" t="inlineStr">
+      <c r="Q46" t="inlineStr">
         <is>
           <t>7/6/22 16:54</t>
         </is>
       </c>
-      <c r="V46" t="n">
-        <v>0</v>
-      </c>
-      <c r="W46" t="inlineStr">
+      <c r="R46" t="n">
+        <v>0</v>
+      </c>
+      <c r="S46" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -4350,59 +3502,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G47" t="inlineStr"/>
-      <c r="H47" t="inlineStr"/>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J47" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L47" t="inlineStr"/>
-      <c r="M47" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N47" t="n">
+      <c r="J47" t="n">
         <v>12</v>
       </c>
+      <c r="K47" t="n">
+        <v>12</v>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O47" t="n">
-        <v>12</v>
-      </c>
-      <c r="P47" t="inlineStr"/>
-      <c r="Q47" t="inlineStr"/>
-      <c r="R47" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S47" t="n">
         <v>100</v>
       </c>
-      <c r="T47" t="inlineStr">
+      <c r="P47" t="inlineStr">
         <is>
           <t>North Macedonia</t>
         </is>
       </c>
-      <c r="U47" t="inlineStr">
+      <c r="Q47" t="inlineStr">
         <is>
           <t>7/6/22 16:50</t>
         </is>
       </c>
-      <c r="V47" t="n">
-        <v>0</v>
-      </c>
-      <c r="W47" t="inlineStr">
+      <c r="R47" t="n">
+        <v>0</v>
+      </c>
+      <c r="S47" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -4435,59 +3572,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G48" t="inlineStr"/>
-      <c r="H48" t="inlineStr"/>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L48" t="inlineStr"/>
-      <c r="M48" t="inlineStr">
-        <is>
           <t>Elvis Week Legacy Pass- 5 Live Legacy Pass Events + 1 Week VOD Each - $130 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N48" t="n">
+      <c r="J48" t="n">
         <v>11</v>
       </c>
+      <c r="K48" t="n">
+        <v>11</v>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O48" t="n">
-        <v>11</v>
-      </c>
-      <c r="P48" t="inlineStr"/>
-      <c r="Q48" t="inlineStr"/>
-      <c r="R48" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S48" t="n">
         <v>100</v>
       </c>
-      <c r="T48" t="inlineStr">
+      <c r="P48" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U48" t="inlineStr">
+      <c r="Q48" t="inlineStr">
         <is>
           <t>7/6/22 16:38</t>
         </is>
       </c>
-      <c r="V48" t="n">
-        <v>0</v>
-      </c>
-      <c r="W48" t="inlineStr">
+      <c r="R48" t="n">
+        <v>0</v>
+      </c>
+      <c r="S48" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -4520,59 +3642,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G49" t="inlineStr"/>
-      <c r="H49" t="inlineStr"/>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L49" t="inlineStr"/>
-      <c r="M49" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N49" t="n">
+      <c r="J49" t="n">
         <v>10</v>
       </c>
+      <c r="K49" t="n">
+        <v>10</v>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O49" t="n">
-        <v>10</v>
-      </c>
-      <c r="P49" t="inlineStr"/>
-      <c r="Q49" t="inlineStr"/>
-      <c r="R49" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S49" t="n">
         <v>100</v>
       </c>
-      <c r="T49" t="inlineStr">
+      <c r="P49" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U49" t="inlineStr">
+      <c r="Q49" t="inlineStr">
         <is>
           <t>7/6/22 16:08</t>
         </is>
       </c>
-      <c r="V49" t="n">
-        <v>0</v>
-      </c>
-      <c r="W49" t="inlineStr">
+      <c r="R49" t="n">
+        <v>0</v>
+      </c>
+      <c r="S49" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -4605,59 +3712,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G50" t="inlineStr"/>
-      <c r="H50" t="inlineStr"/>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L50" t="inlineStr"/>
-      <c r="M50" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N50" t="n">
+      <c r="J50" t="n">
         <v>9</v>
       </c>
+      <c r="K50" t="n">
+        <v>9</v>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O50" t="n">
-        <v>9</v>
-      </c>
-      <c r="P50" t="inlineStr"/>
-      <c r="Q50" t="inlineStr"/>
-      <c r="R50" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S50" t="n">
         <v>100</v>
       </c>
-      <c r="T50" t="inlineStr">
+      <c r="P50" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U50" t="inlineStr">
+      <c r="Q50" t="inlineStr">
         <is>
           <t>7/6/22 15:33</t>
         </is>
       </c>
-      <c r="V50" t="n">
-        <v>0</v>
-      </c>
-      <c r="W50" t="inlineStr">
+      <c r="R50" t="n">
+        <v>0</v>
+      </c>
+      <c r="S50" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -4690,59 +3782,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G51" t="inlineStr"/>
-      <c r="H51" t="inlineStr"/>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L51" t="inlineStr"/>
-      <c r="M51" t="inlineStr">
-        <is>
           <t>Elvis Week Legacy Pass- 5 Live Legacy Pass Events + 1 Week VOD Each - $130 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N51" t="n">
+      <c r="J51" t="n">
         <v>8</v>
       </c>
+      <c r="K51" t="n">
+        <v>8</v>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O51" t="n">
-        <v>8</v>
-      </c>
-      <c r="P51" t="inlineStr"/>
-      <c r="Q51" t="inlineStr"/>
-      <c r="R51" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S51" t="n">
         <v>100</v>
       </c>
-      <c r="T51" t="inlineStr">
+      <c r="P51" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U51" t="inlineStr">
+      <c r="Q51" t="inlineStr">
         <is>
           <t>7/6/22 15:30</t>
         </is>
       </c>
-      <c r="V51" t="n">
-        <v>0</v>
-      </c>
-      <c r="W51" t="inlineStr">
+      <c r="R51" t="n">
+        <v>0</v>
+      </c>
+      <c r="S51" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -4775,59 +3852,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G52" t="inlineStr"/>
-      <c r="H52" t="inlineStr"/>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L52" t="inlineStr"/>
-      <c r="M52" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N52" t="n">
+      <c r="J52" t="n">
         <v>7</v>
       </c>
+      <c r="K52" t="n">
+        <v>7</v>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O52" t="n">
-        <v>7</v>
-      </c>
-      <c r="P52" t="inlineStr"/>
-      <c r="Q52" t="inlineStr"/>
-      <c r="R52" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S52" t="n">
         <v>100</v>
       </c>
-      <c r="T52" t="inlineStr">
+      <c r="P52" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U52" t="inlineStr">
+      <c r="Q52" t="inlineStr">
         <is>
           <t>7/6/22 13:44</t>
         </is>
       </c>
-      <c r="V52" t="n">
-        <v>0</v>
-      </c>
-      <c r="W52" t="inlineStr">
+      <c r="R52" t="n">
+        <v>0</v>
+      </c>
+      <c r="S52" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -4860,59 +3922,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G53" t="inlineStr"/>
-      <c r="H53" t="inlineStr"/>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J53" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L53" t="inlineStr"/>
-      <c r="M53" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N53" t="n">
+      <c r="J53" t="n">
         <v>6</v>
       </c>
+      <c r="K53" t="n">
+        <v>6</v>
+      </c>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O53" t="n">
-        <v>6</v>
-      </c>
-      <c r="P53" t="inlineStr"/>
-      <c r="Q53" t="inlineStr"/>
-      <c r="R53" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S53" t="n">
         <v>100</v>
       </c>
-      <c r="T53" t="inlineStr">
+      <c r="P53" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U53" t="inlineStr">
+      <c r="Q53" t="inlineStr">
         <is>
           <t>7/6/22 4:41</t>
         </is>
       </c>
-      <c r="V53" t="n">
-        <v>0</v>
-      </c>
-      <c r="W53" t="inlineStr">
+      <c r="R53" t="n">
+        <v>0</v>
+      </c>
+      <c r="S53" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -4945,59 +3992,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G54" t="inlineStr"/>
-      <c r="H54" t="inlineStr"/>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J54" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L54" t="inlineStr"/>
-      <c r="M54" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N54" t="n">
+      <c r="J54" t="n">
         <v>5</v>
       </c>
+      <c r="K54" t="n">
+        <v>5</v>
+      </c>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O54" t="n">
-        <v>5</v>
-      </c>
-      <c r="P54" t="inlineStr"/>
-      <c r="Q54" t="inlineStr"/>
-      <c r="R54" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S54" t="n">
         <v>100</v>
       </c>
-      <c r="T54" t="inlineStr">
+      <c r="P54" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U54" t="inlineStr">
+      <c r="Q54" t="inlineStr">
         <is>
           <t>7/6/22 4:38</t>
         </is>
       </c>
-      <c r="V54" t="n">
-        <v>0</v>
-      </c>
-      <c r="W54" t="inlineStr">
+      <c r="R54" t="n">
+        <v>0</v>
+      </c>
+      <c r="S54" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -5030,59 +4062,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G55" t="inlineStr"/>
-      <c r="H55" t="inlineStr"/>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J55" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L55" t="inlineStr"/>
-      <c r="M55" t="inlineStr">
-        <is>
           <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N55" t="n">
+      <c r="J55" t="n">
         <v>4</v>
       </c>
+      <c r="K55" t="n">
+        <v>4</v>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O55" t="n">
-        <v>4</v>
-      </c>
-      <c r="P55" t="inlineStr"/>
-      <c r="Q55" t="inlineStr"/>
-      <c r="R55" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S55" t="n">
         <v>100</v>
       </c>
-      <c r="T55" t="inlineStr">
+      <c r="P55" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U55" t="inlineStr">
+      <c r="Q55" t="inlineStr">
         <is>
           <t>7/5/22 21:31</t>
         </is>
       </c>
-      <c r="V55" t="n">
-        <v>0</v>
-      </c>
-      <c r="W55" t="inlineStr">
+      <c r="R55" t="n">
+        <v>0</v>
+      </c>
+      <c r="S55" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -5115,59 +4132,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G56" t="inlineStr"/>
-      <c r="H56" t="inlineStr"/>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L56" t="inlineStr"/>
-      <c r="M56" t="inlineStr">
-        <is>
           <t>Elvis Week Tribute Pass- 4 Live Tribute Pass Events + 1 Week  VOD Each - $130 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N56" t="n">
+      <c r="J56" t="n">
         <v>3</v>
       </c>
+      <c r="K56" t="n">
+        <v>3</v>
+      </c>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O56" t="n">
-        <v>3</v>
-      </c>
-      <c r="P56" t="inlineStr"/>
-      <c r="Q56" t="inlineStr"/>
-      <c r="R56" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S56" t="n">
         <v>100</v>
       </c>
-      <c r="T56" t="inlineStr">
+      <c r="P56" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U56" t="inlineStr">
+      <c r="Q56" t="inlineStr">
         <is>
           <t>7/5/22 21:30</t>
         </is>
       </c>
-      <c r="V56" t="n">
-        <v>0</v>
-      </c>
-      <c r="W56" t="inlineStr">
+      <c r="R56" t="n">
+        <v>0</v>
+      </c>
+      <c r="S56" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -5200,59 +4202,44 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G57" t="inlineStr"/>
-      <c r="H57" t="inlineStr"/>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J57" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>Used voucher VoucherName (voucherCode),</t>
-        </is>
-      </c>
-      <c r="L57" t="inlineStr"/>
-      <c r="M57" t="inlineStr">
-        <is>
           <t>Elvis Week Legacy Pass- 5 Live Legacy Pass Events + 1 Week VOD Each - $130 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N57" t="n">
+      <c r="J57" t="n">
         <v>2</v>
       </c>
+      <c r="K57" t="n">
+        <v>2</v>
+      </c>
+      <c r="N57" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
       <c r="O57" t="n">
-        <v>2</v>
-      </c>
-      <c r="P57" t="inlineStr"/>
-      <c r="Q57" t="inlineStr"/>
-      <c r="R57" t="inlineStr">
-        <is>
-          <t>voucherCode</t>
-        </is>
-      </c>
-      <c r="S57" t="n">
         <v>100</v>
       </c>
-      <c r="T57" t="inlineStr">
+      <c r="P57" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U57" t="inlineStr">
+      <c r="Q57" t="inlineStr">
         <is>
           <t>7/5/22 20:45</t>
         </is>
       </c>
-      <c r="V57" t="n">
-        <v>0</v>
-      </c>
-      <c r="W57" t="inlineStr">
+      <c r="R57" t="n">
+        <v>0</v>
+      </c>
+      <c r="S57" t="inlineStr">
         <is>
           <t>voucherCode</t>
         </is>
@@ -5285,57 +4272,36 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="G58" t="n">
-        <v>4.62</v>
-      </c>
-      <c r="H58" t="n">
-        <v>127.38</v>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>https://virtualelvisweek.com/dev/artisttribute/index.html</t>
+        </is>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>charge</t>
-        </is>
-      </c>
-      <c r="J58" t="inlineStr">
-        <is>
-          <t>Stripe</t>
-        </is>
-      </c>
-      <c r="K58" t="inlineStr"/>
-      <c r="L58" t="inlineStr">
-        <is>
-          <t>https://virtualelvisweek.com/dev/artisttribute/index.html</t>
-        </is>
-      </c>
-      <c r="M58" t="inlineStr">
-        <is>
           <t>Elvis Week Tribute Pass- 4 Live Tribute Pass Events + 1 Week  VOD Each - $130 + $2 Processing Fee</t>
         </is>
       </c>
-      <c r="N58" t="n">
+      <c r="J58" t="n">
         <v>1</v>
       </c>
-      <c r="O58" t="n">
+      <c r="K58" t="n">
         <v>1</v>
       </c>
-      <c r="P58" t="inlineStr"/>
-      <c r="Q58" t="inlineStr"/>
-      <c r="R58" t="inlineStr"/>
-      <c r="S58" t="inlineStr"/>
-      <c r="T58" t="inlineStr">
+      <c r="P58" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="U58" t="inlineStr">
+      <c r="Q58" t="inlineStr">
         <is>
           <t>6/30/22 17:19</t>
         </is>
       </c>
-      <c r="V58" t="n">
-        <v>0</v>
-      </c>
-      <c r="W58" t="inlineStr">
+      <c r="R58" t="n">
+        <v>0</v>
+      </c>
+      <c r="S58" t="inlineStr">
         <is>
           <t>ch_</t>
         </is>
@@ -5344,4 +4310,58 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
voucher/refund tabs, adds heading row to all new sheets
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -4318,14 +4318,23 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="2"/>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -4336,14 +4345,23 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="2"/>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -4354,14 +4372,23 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="2"/>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>